<commit_message>
added new XGB submission
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABF700E-06FF-E54B-B4FB-F0310B08F68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D16F67-DB64-6648-BCB5-F9590B66C677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17300" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Melo_Stoelben_Test</t>
+  </si>
+  <si>
+    <t>221118_xgb_external</t>
+  </si>
+  <si>
+    <t>6_JM_MS</t>
   </si>
 </sst>
 </file>
@@ -153,8 +159,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -463,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="222" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,6 +577,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>44883</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added to tuned xgb submissions
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D16F67-DB64-6648-BCB5-F9590B66C677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC13058-C63A-174F-99C8-7C37CED4E3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -99,6 +99,18 @@
   </si>
   <si>
     <t>6_JM_MS</t>
+  </si>
+  <si>
+    <t>7_JM_MS</t>
+  </si>
+  <si>
+    <t>8_JM_MS</t>
+  </si>
+  <si>
+    <t>221120_xgb_tuned</t>
+  </si>
+  <si>
+    <t>221121_xgb_tuned</t>
   </si>
 </sst>
 </file>
@@ -159,8 +171,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E7" totalsRowShown="0">
-  <autoFilter ref="A1:E7" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E9" totalsRowShown="0">
+  <autoFilter ref="A1:E9" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -469,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="222" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,6 +606,40 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>44885</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>44886</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added new submissions to tracker
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC13058-C63A-174F-99C8-7C37CED4E3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDB91E1-654A-E94A-935B-33B482013616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -111,6 +111,27 @@
   </si>
   <si>
     <t>221121_xgb_tuned</t>
+  </si>
+  <si>
+    <t>9_JM_MS</t>
+  </si>
+  <si>
+    <t>10_JM_MS</t>
+  </si>
+  <si>
+    <t>11_JM_MS</t>
+  </si>
+  <si>
+    <t>221123_xgb_reduced_2</t>
+  </si>
+  <si>
+    <t>221123_ligthgbm</t>
+  </si>
+  <si>
+    <t>221122_xgb_reduced</t>
+  </si>
+  <si>
+    <t>12_JM_MS</t>
   </si>
 </sst>
 </file>
@@ -171,8 +192,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E9" totalsRowShown="0">
-  <autoFilter ref="A1:E9" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E13" totalsRowShown="0">
+  <autoFilter ref="A1:E13" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -481,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="222" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,6 +661,71 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>44887</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>44888</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>44888</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>44888</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added all folders of submission to excel
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDB91E1-654A-E94A-935B-33B482013616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C09BAA-0A34-1D46-979B-106A7E444E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -132,6 +132,24 @@
   </si>
   <si>
     <t>12_JM_MS</t>
+  </si>
+  <si>
+    <t>221123_cat_monkey</t>
+  </si>
+  <si>
+    <t>221123_cat</t>
+  </si>
+  <si>
+    <t>test_bis_JM_MS</t>
+  </si>
+  <si>
+    <t>test_JM_MS</t>
+  </si>
+  <si>
+    <t>221122_ET</t>
+  </si>
+  <si>
+    <t>221123_xgb_reduced_3</t>
   </si>
 </sst>
 </file>
@@ -192,8 +210,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E13" totalsRowShown="0">
-  <autoFilter ref="A1:E13" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E16" totalsRowShown="0">
+  <autoFilter ref="A1:E16" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -502,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="222" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,6 +734,9 @@
       <c r="A13" s="1">
         <v>44888</v>
       </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
       <c r="C13" t="s">
         <v>31</v>
       </c>
@@ -724,6 +745,51 @@
       </c>
       <c r="E13" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>44888</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>44889</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added submissions for tuned cat and cat_monkey
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C09BAA-0A34-1D46-979B-106A7E444E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8803C88F-98BB-214B-A314-6492B6707BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>221123_xgb_reduced_3</t>
+  </si>
+  <si>
+    <t>221125_cat_tuning</t>
+  </si>
+  <si>
+    <t>221125_cat_monkey_tuning</t>
+  </si>
+  <si>
+    <t>droelf_JM_MS</t>
   </si>
 </sst>
 </file>
@@ -210,8 +219,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E16" totalsRowShown="0">
-  <autoFilter ref="A1:E16" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E18" totalsRowShown="0">
+  <autoFilter ref="A1:E18" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -520,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="177" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -792,6 +801,34 @@
         <v>9</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>44890</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added new cat tuning results unrestricted learning rate and new submission
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8803C88F-98BB-214B-A314-6492B6707BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDF1ACC-1EF9-6646-815E-DBF8F96C4928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>droelf_JM_MS</t>
+  </si>
+  <si>
+    <t>herewegoagain_JM_MS</t>
+  </si>
+  <si>
+    <t>221125_cat_tuning_2</t>
   </si>
 </sst>
 </file>
@@ -219,8 +225,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E18" totalsRowShown="0">
-  <autoFilter ref="A1:E18" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E19" totalsRowShown="0">
+  <autoFilter ref="A1:E19" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -529,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="177" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -829,6 +835,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>44890</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added new cat tuning submissions on the 26.11.
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDF1ACC-1EF9-6646-815E-DBF8F96C4928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44AD6C1-6901-3C4E-A426-6D12F549CDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -165,6 +165,30 @@
   </si>
   <si>
     <t>221125_cat_tuning_2</t>
+  </si>
+  <si>
+    <t>221126_cat_tuning_3</t>
+  </si>
+  <si>
+    <t>221126_cat_tuning_4</t>
+  </si>
+  <si>
+    <t>221126_cat_tuning_5</t>
+  </si>
+  <si>
+    <t>221126_cat_tuning_6</t>
+  </si>
+  <si>
+    <t>deep_neural_nada</t>
+  </si>
+  <si>
+    <t>japanese_chalk</t>
+  </si>
+  <si>
+    <t>japanese_chalk_2</t>
+  </si>
+  <si>
+    <t>Logistic_Regression</t>
   </si>
 </sst>
 </file>
@@ -225,8 +249,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E19" totalsRowShown="0">
-  <autoFilter ref="A1:E19" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E23" totalsRowShown="0">
+  <autoFilter ref="A1:E23" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -535,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="177" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,6 +876,74 @@
         <v>10</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>44891</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>44891</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>44891</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>44891</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added new submission to test feature processing
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44AD6C1-6901-3C4E-A426-6D12F549CDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBC794C-8E8F-8C49-B68B-D892C21597AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>Logistic_Regression</t>
+  </si>
+  <si>
+    <t>NewPhoneWhoDis</t>
+  </si>
+  <si>
+    <t>221126_cat_test</t>
   </si>
 </sst>
 </file>
@@ -249,8 +255,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E23" totalsRowShown="0">
-  <autoFilter ref="A1:E23" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E24" totalsRowShown="0">
+  <autoFilter ref="A1:E24" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -559,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="177" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,6 +950,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>44891</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added new submission with longitude and latitude
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBC794C-8E8F-8C49-B68B-D892C21597AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4934CB65-9F89-0645-A6E6-263D2E8FD3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>221126_cat_test</t>
+  </si>
+  <si>
+    <t>221126_cat_test_2</t>
+  </si>
+  <si>
+    <t>pineapple_pizza</t>
   </si>
 </sst>
 </file>
@@ -255,8 +261,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E24" totalsRowShown="0">
-  <autoFilter ref="A1:E24" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E25" totalsRowShown="0">
+  <autoFilter ref="A1:E25" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -565,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="177" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,6 +973,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>44891</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added submission and tuning results after feature processing, before adding lon/lat
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4934CB65-9F89-0645-A6E6-263D2E8FD3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AD4BBC-28C5-5B41-A9D6-C41EA5AC236B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>pineapple_pizza</t>
+  </si>
+  <si>
+    <t>78LaundryIsDone</t>
+  </si>
+  <si>
+    <t>221126_cat_v1data</t>
   </si>
 </sst>
 </file>
@@ -261,8 +267,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E25" totalsRowShown="0">
-  <autoFilter ref="A1:E25" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E26" totalsRowShown="0">
+  <autoFilter ref="A1:E26" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -571,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="177" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -990,6 +996,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>44891</v>
+      </c>
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added new submissions of cat tuning
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AD4BBC-28C5-5B41-A9D6-C41EA5AC236B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C0835B-B996-134B-8FA2-F1267D0BBB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -207,6 +207,18 @@
   </si>
   <si>
     <t>221126_cat_v1data</t>
+  </si>
+  <si>
+    <t>trial_JM_MS</t>
+  </si>
+  <si>
+    <t>mangan_steakNfries</t>
+  </si>
+  <si>
+    <t>221127_cat_v2data_deeper</t>
+  </si>
+  <si>
+    <t>221127_cat_v2data</t>
   </si>
 </sst>
 </file>
@@ -267,8 +279,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E26" totalsRowShown="0">
-  <autoFilter ref="A1:E26" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E28" totalsRowShown="0">
+  <autoFilter ref="A1:E28" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -577,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="177" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1013,6 +1025,40 @@
         <v>10</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>44892</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>44892</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
black encoded submissions and added final tuned ones for xgb, cat, lightgbm
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C0835B-B996-134B-8FA2-F1267D0BBB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50422BC-EEA7-6F42-A390-BC6885985430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -219,6 +219,24 @@
   </si>
   <si>
     <t>221127_cat_v2data</t>
+  </si>
+  <si>
+    <t>version_1_1</t>
+  </si>
+  <si>
+    <t>version_1_2</t>
+  </si>
+  <si>
+    <t>version_1_3</t>
+  </si>
+  <si>
+    <t>221127_cat_v2data_final</t>
+  </si>
+  <si>
+    <t>221127_xgb_v2data_final</t>
+  </si>
+  <si>
+    <t>221127_lightgbm_v2data_final</t>
   </si>
 </sst>
 </file>
@@ -279,8 +297,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E28" totalsRowShown="0">
-  <autoFilter ref="A1:E28" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E33" totalsRowShown="0">
+  <autoFilter ref="A1:E33" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -589,15 +607,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="177" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="177" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1058,6 +1076,63 @@
       <c r="E28" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>44892</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>44892</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>44892</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added submission for voting regressor
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50422BC-EEA7-6F42-A390-BC6885985430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEEEDBF-9EF3-F548-A968-7C0613C047BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -227,9 +227,6 @@
     <t>version_1_2</t>
   </si>
   <si>
-    <t>version_1_3</t>
-  </si>
-  <si>
     <t>221127_cat_v2data_final</t>
   </si>
   <si>
@@ -237,6 +234,12 @@
   </si>
   <si>
     <t>221127_lightgbm_v2data_final</t>
+  </si>
+  <si>
+    <t>221127_voting_regressor</t>
+  </si>
+  <si>
+    <t>last_but_not_best</t>
   </si>
 </sst>
 </file>
@@ -609,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="177" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1082,7 +1085,7 @@
         <v>44892</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
         <v>61</v>
@@ -1099,7 +1102,7 @@
         <v>44892</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
         <v>62</v>
@@ -1116,20 +1119,31 @@
         <v>44892</v>
       </c>
       <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>44892</v>
+      </c>
+      <c r="B32" t="s">
         <v>66</v>
       </c>
-      <c r="C31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>

</xml_diff>

<commit_message>
added new trials for submission with more covid data
</commit_message>
<xml_diff>
--- a/submissions/Submission_tracker.xlsx
+++ b/submissions/Submission_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/HS22/Python_for_Data_Science/bike_counters/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEEEDBF-9EF3-F548-A968-7C0613C047BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1852A79E-695B-8D4E-9F81-D514E184760C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="17340" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="10440" windowHeight="17200" xr2:uid="{2D72A904-ABCE-1048-B376-D24C1C1684B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -240,6 +240,78 @@
   </si>
   <si>
     <t>last_but_not_best</t>
+  </si>
+  <si>
+    <t>221129_final_model</t>
+  </si>
+  <si>
+    <t>final_model</t>
+  </si>
+  <si>
+    <t>final_model_v2</t>
+  </si>
+  <si>
+    <t>221129_final_model_v2</t>
+  </si>
+  <si>
+    <t>test_new_data</t>
+  </si>
+  <si>
+    <t>model_name</t>
+  </si>
+  <si>
+    <t>model_name_2</t>
+  </si>
+  <si>
+    <t>14_gewinnt</t>
+  </si>
+  <si>
+    <t>caca_aos_gambuzinos</t>
+  </si>
+  <si>
+    <t>estimator_1</t>
+  </si>
+  <si>
+    <t>estimator_2</t>
+  </si>
+  <si>
+    <t>estimator_3</t>
+  </si>
+  <si>
+    <t>estimator_4</t>
+  </si>
+  <si>
+    <t>estimator_5</t>
+  </si>
+  <si>
+    <t>estimaror_6</t>
+  </si>
+  <si>
+    <t>221130_best_grid</t>
+  </si>
+  <si>
+    <t>221130_lowest_test</t>
+  </si>
+  <si>
+    <t>221129_test_new_data</t>
+  </si>
+  <si>
+    <t>221129_test_new_data_2</t>
+  </si>
+  <si>
+    <t>221129_test_new_data_3</t>
+  </si>
+  <si>
+    <t>221129_test_new_data_4</t>
+  </si>
+  <si>
+    <t>221129_test_new_data_5</t>
+  </si>
+  <si>
+    <t>221129_test_new_data_6</t>
+  </si>
+  <si>
+    <t>221129_test_new_data_7</t>
   </si>
 </sst>
 </file>
@@ -300,8 +372,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E33" totalsRowShown="0">
-  <autoFilter ref="A1:E33" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}" name="Tabelle2" displayName="Tabelle2" ref="A1:E45" totalsRowShown="0">
+  <autoFilter ref="A1:E45" xr:uid="{A7BE2D84-B706-D047-8878-1A5586460BE8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{155D9DEA-9897-7E4E-9F25-35232AB43CB5}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{574842E6-199D-354B-A479-1323C9D03E56}" name="Name"/>
@@ -610,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16051AA7-1978-BE4B-B9A6-112D76F7500E}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1145,8 +1217,226 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>44894</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>44894</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>44894</v>
+      </c>
+      <c r="B35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>44894</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>44894</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>44894</v>
+      </c>
+      <c r="B38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>44894</v>
+      </c>
+      <c r="B39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>44894</v>
+      </c>
+      <c r="B40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>44894</v>
+      </c>
+      <c r="B41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>44894</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>44894</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>44895</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>44895</v>
+      </c>
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>